<commit_message>
anik fixed impariment entry
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/sample/Impairment_data.xlsx
+++ b/afar_project/csv_path/sample/Impairment_data.xlsx
@@ -1087,10 +1087,10 @@
         <v>4822.65</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="V8" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
anik fixed impairment touple isse
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/sample/Impairment_data.xlsx
+++ b/afar_project/csv_path/sample/Impairment_data.xlsx
@@ -1007,10 +1007,10 @@
         <v>1747.95</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
anik fixed afar_project Views
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/sample/Impairment_data.xlsx
+++ b/afar_project/csv_path/sample/Impairment_data.xlsx
@@ -476,22 +476,22 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Book_Value</t>
+          <t>Book Value</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Fair_value_less_cost_to_sale</t>
+          <t>Fair value less cost to sale</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Value_in_use</t>
+          <t>Value in use</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Recoverable Amount</t>
+          <t>Recoverable Value</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0001</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0002</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -640,7 +640,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0003</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -693,7 +693,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0004</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0005</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -799,7 +799,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0006</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -852,7 +852,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0007</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -903,7 +903,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0008</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -954,7 +954,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0009</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>FRC-7-C-17-0000</t>
+          <t>FRC-HQ-SLM-C-17-0010</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>FRC-7-C-17-0000</t>
+          <t>FRC-HQ-SLM-C-17-0011</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0012</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0013</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0014</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0015</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0016</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0017</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0018</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0019</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0020</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0021</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0022</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0023</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0024</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0025</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0026</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0027</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0028</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0029</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0030</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0031</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0032</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0033</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0034</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0035</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0036</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0037</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0038</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0039</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0040</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0041</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0042</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0043</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0044</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>FRC-7-T-18-0000</t>
+          <t>FRC-HQ-SLM-T-18-0045</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>FRC-7-T-18-0000</t>
+          <t>FRC-HQ-SLM-T-18-0046</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0047</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0048</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -3050,7 +3050,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0049</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>FRC-7-O-17-0000</t>
+          <t>FRC-HQ-SLM-O-17-0050</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0051</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0052</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -3262,7 +3262,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>FRC-7-F-17-0000</t>
+          <t>FRC-HQ-SLM-F-17-0053</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0054</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0055</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0056</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -3474,7 +3474,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0057</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0058</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0059</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0060</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0061</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -3735,7 +3735,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0062</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0063</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0064</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0065</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0066</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0067</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -4051,7 +4051,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0068</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -4104,7 +4104,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0069</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0070</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0071</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0072</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0073</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0074</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0075</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>FRC-7-T-18-0000</t>
+          <t>FRC-HQ-SLM-T-18-0076</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0000</t>
+          <t>FRC-HQ-SLM-F-19-0077</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -4579,7 +4579,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0078</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0079</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -4683,7 +4683,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0080</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0081</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0082</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -4842,7 +4842,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0083</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0084</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0085</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0086</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -5050,7 +5050,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0000</t>
+          <t>FRC-HQ-SLM-O-18-0087</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0088</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -5154,7 +5154,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0089</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -5207,7 +5207,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>FRC-7-C-18-0000</t>
+          <t>FRC-HQ-SLM-C-18-0090</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -5260,7 +5260,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0091</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0092</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0093</t>
         </is>
       </c>
       <c r="I94" t="n">
@@ -5419,7 +5419,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0000</t>
+          <t>FRC-HQ-SLM-O-19-0094</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -5472,7 +5472,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>FRC-7-F-18-0000</t>
+          <t>FRC-HQ-SLM-F-18-0095</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0000</t>
+          <t>FRC-HQ-SLM-O-19-0096</t>
         </is>
       </c>
       <c r="I97" t="n">
@@ -5576,7 +5576,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>FRC-7-T-19-0000</t>
+          <t>FRC-HQ-SLM-T-19-0097</t>
         </is>
       </c>
       <c r="I98" t="n">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>FRC-7-M-19-0000</t>
+          <t>FRC-HQ-SLM-M-19-0098</t>
         </is>
       </c>
       <c r="I99" t="n">
@@ -5682,7 +5682,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>FRC-7-M-19-0000</t>
+          <t>FRC-HQ-SLM-M-19-0099</t>
         </is>
       </c>
       <c r="I100" t="n">
@@ -5733,7 +5733,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0100</t>
         </is>
       </c>
       <c r="I101" t="n">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0101</t>
         </is>
       </c>
       <c r="I102" t="n">
@@ -5835,7 +5835,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0102</t>
         </is>
       </c>
       <c r="I103" t="n">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0103</t>
         </is>
       </c>
       <c r="I104" t="n">
@@ -5939,7 +5939,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0104</t>
         </is>
       </c>
       <c r="I105" t="n">
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0105</t>
         </is>
       </c>
       <c r="I106" t="n">
@@ -6045,7 +6045,7 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>FRC-7-O-18-0001</t>
+          <t>FRC-HQ-SLM-O-18-0106</t>
         </is>
       </c>
       <c r="I107" t="n">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0107</t>
         </is>
       </c>
       <c r="I108" t="n">
@@ -6151,7 +6151,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0108</t>
         </is>
       </c>
       <c r="I109" t="n">
@@ -6202,7 +6202,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0109</t>
         </is>
       </c>
       <c r="I110" t="n">
@@ -6255,7 +6255,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0110</t>
         </is>
       </c>
       <c r="I111" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0111</t>
         </is>
       </c>
       <c r="I112" t="n">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>FRC-7-F-20-0001</t>
+          <t>FRC-HQ-SLM-F-20-0112</t>
         </is>
       </c>
       <c r="I113" t="n">
@@ -6414,7 +6414,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0113</t>
         </is>
       </c>
       <c r="I114" t="n">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0114</t>
         </is>
       </c>
       <c r="I115" t="n">
@@ -6520,7 +6520,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0115</t>
         </is>
       </c>
       <c r="I116" t="n">
@@ -6573,7 +6573,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0116</t>
         </is>
       </c>
       <c r="I117" t="n">
@@ -6626,7 +6626,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0117</t>
         </is>
       </c>
       <c r="I118" t="n">
@@ -6679,7 +6679,7 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0118</t>
         </is>
       </c>
       <c r="I119" t="n">
@@ -6732,7 +6732,7 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0119</t>
         </is>
       </c>
       <c r="I120" t="n">
@@ -6785,7 +6785,7 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>FRC-7-O-19-0001</t>
+          <t>FRC-HQ-SLM-O-19-0120</t>
         </is>
       </c>
       <c r="I121" t="n">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>FRC-7-F-19-0001</t>
+          <t>FRC-HQ-SLM-F-19-0121</t>
         </is>
       </c>
       <c r="I122" t="n">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>FRC-7-C-19-0001</t>
+          <t>FRC-HQ-SLM-C-19-0122</t>
         </is>
       </c>
       <c r="I123" t="n">
@@ -6944,7 +6944,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>FRC-7-C-19-0001</t>
+          <t>FRC-HQ-SLM-C-19-0123</t>
         </is>
       </c>
       <c r="I124" t="n">
@@ -6997,7 +6997,7 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>FRC-7-C-19-0001</t>
+          <t>FRC-HQ-SLM-C-19-0124</t>
         </is>
       </c>
       <c r="I125" t="n">
@@ -7048,7 +7048,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>FRC-7-C-19-0001</t>
+          <t>FRC-HQ-SLM-C-19-0125</t>
         </is>
       </c>
       <c r="I126" t="n">
@@ -7101,7 +7101,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>FRC-7-F-20-0001</t>
+          <t>FRC-HQ-SLM-F-20-0126</t>
         </is>
       </c>
       <c r="I127" t="n">
@@ -7154,7 +7154,7 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>FRC-7-F-20-0001</t>
+          <t>FRC-HQ-SLM-F-20-0127</t>
         </is>
       </c>
       <c r="I128" t="n">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>FRC-7-F-20-0001</t>
+          <t>FRC-HQ-SLM-F-20-0128</t>
         </is>
       </c>
       <c r="I129" t="n">
@@ -7260,7 +7260,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>FRC-7-C-20-0001</t>
+          <t>FRC-HQ-SLM-C-20-0129</t>
         </is>
       </c>
       <c r="I130" t="n">
@@ -7313,7 +7313,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>FRC-7-C-20-0001</t>
+          <t>FRC-HQ-SLM-C-20-0130</t>
         </is>
       </c>
       <c r="I131" t="n">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>FRC-7-C-20-0001</t>
+          <t>FRC-HQ-SLM-C-20-0131</t>
         </is>
       </c>
       <c r="I132" t="n">
@@ -7419,7 +7419,7 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>FRC-7-C-20-0001</t>
+          <t>FRC-HQ-SLM-C-20-0132</t>
         </is>
       </c>
       <c r="I133" t="n">
@@ -7472,7 +7472,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>FRC-7-T-20-0001</t>
+          <t>FRC-HQ-SLM-T-20-0133</t>
         </is>
       </c>
       <c r="I134" t="n">
@@ -7525,7 +7525,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0134</t>
         </is>
       </c>
       <c r="I135" t="n">
@@ -7578,7 +7578,7 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0135</t>
         </is>
       </c>
       <c r="I136" t="n">
@@ -7629,7 +7629,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0136</t>
         </is>
       </c>
       <c r="I137" t="n">
@@ -7682,7 +7682,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0137</t>
         </is>
       </c>
       <c r="I138" t="n">
@@ -7735,7 +7735,7 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>FRC-7-F-21-0001</t>
+          <t>FRC-HQ-SLM-F-21-0138</t>
         </is>
       </c>
       <c r="I139" t="n">
@@ -7788,7 +7788,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0139</t>
         </is>
       </c>
       <c r="I140" t="n">
@@ -7841,7 +7841,7 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>FRC-7-F-21-0001</t>
+          <t>FRC-HQ-SLM-F-21-0140</t>
         </is>
       </c>
       <c r="I141" t="n">
@@ -7894,7 +7894,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0141</t>
         </is>
       </c>
       <c r="I142" t="n">
@@ -7947,7 +7947,7 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>FRC-7-C-21-0001</t>
+          <t>FRC-HQ-SLM-C-21-0142</t>
         </is>
       </c>
       <c r="I143" t="n">
@@ -8000,7 +8000,7 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>FRC-7-M-21-0001</t>
+          <t>FRC-HQ-SLM-M-21-0143</t>
         </is>
       </c>
       <c r="I144" t="n">
@@ -8051,7 +8051,7 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>FRC-7-M-21-0001</t>
+          <t>FRC-HQ-SLM-M-21-0144</t>
         </is>
       </c>
       <c r="I145" t="n">
@@ -8104,7 +8104,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>FRC-7-O-22-0001</t>
+          <t>FRC-HQ-SLM-O-22-0145</t>
         </is>
       </c>
       <c r="I146" t="n">
@@ -8157,7 +8157,7 @@
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0146</t>
         </is>
       </c>
       <c r="I147" t="n">
@@ -8210,7 +8210,7 @@
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0147</t>
         </is>
       </c>
       <c r="I148" t="n">
@@ -8261,7 +8261,7 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>FRC-7-M-22-0001</t>
+          <t>FRC-HQ-SLM-M-22-0148</t>
         </is>
       </c>
       <c r="I149" t="n">
@@ -8314,7 +8314,7 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0001</t>
+          <t>FRC-HQ-SLM-F-22-0149</t>
         </is>
       </c>
       <c r="I150" t="n">
@@ -8367,7 +8367,7 @@
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>FRC-7-O-22-0001</t>
+          <t>FRC-HQ-SLM-O-22-0150</t>
         </is>
       </c>
       <c r="I151" t="n">
@@ -8418,7 +8418,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0152</t>
         </is>
       </c>
       <c r="I152" t="n">
@@ -8469,7 +8469,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0153</t>
         </is>
       </c>
       <c r="I153" t="n">
@@ -8520,7 +8520,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0154</t>
         </is>
       </c>
       <c r="I154" t="n">
@@ -8571,7 +8571,7 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0155</t>
         </is>
       </c>
       <c r="I155" t="n">
@@ -8622,7 +8622,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0156</t>
         </is>
       </c>
       <c r="I156" t="n">
@@ -8673,7 +8673,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0157</t>
         </is>
       </c>
       <c r="I157" t="n">
@@ -8724,7 +8724,7 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0158</t>
         </is>
       </c>
       <c r="I158" t="n">
@@ -8775,7 +8775,7 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0159</t>
         </is>
       </c>
       <c r="I159" t="n">
@@ -8826,7 +8826,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0160</t>
         </is>
       </c>
       <c r="I160" t="n">
@@ -8877,7 +8877,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>FRC-7-C-22-0001</t>
+          <t>FRC-HQ-SLM-C-22-0161</t>
         </is>
       </c>
       <c r="I161" t="n">
@@ -8928,7 +8928,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0162</t>
         </is>
       </c>
       <c r="I162" t="n">
@@ -8979,7 +8979,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0163</t>
         </is>
       </c>
       <c r="I163" t="n">
@@ -9030,7 +9030,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0164</t>
         </is>
       </c>
       <c r="I164" t="n">
@@ -9081,7 +9081,7 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0165</t>
         </is>
       </c>
       <c r="I165" t="n">
@@ -9132,7 +9132,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0166</t>
         </is>
       </c>
       <c r="I166" t="n">
@@ -9183,7 +9183,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0167</t>
         </is>
       </c>
       <c r="I167" t="n">
@@ -9234,7 +9234,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0168</t>
         </is>
       </c>
       <c r="I168" t="n">
@@ -9286,7 +9286,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0169</t>
         </is>
       </c>
       <c r="I169" t="n">
@@ -9339,7 +9339,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0170</t>
         </is>
       </c>
       <c r="I170" t="n">
@@ -9390,7 +9390,7 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0171</t>
         </is>
       </c>
       <c r="I171" t="n">
@@ -9443,7 +9443,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0001</t>
+          <t>FRC-HQ-SLM-I-22-0172</t>
         </is>
       </c>
       <c r="I172" t="n">
@@ -9496,7 +9496,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0173</t>
         </is>
       </c>
       <c r="I173" t="n">
@@ -9549,7 +9549,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0174</t>
         </is>
       </c>
       <c r="I174" t="n">
@@ -9602,7 +9602,7 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0175</t>
         </is>
       </c>
       <c r="I175" t="n">
@@ -9653,7 +9653,7 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0176</t>
         </is>
       </c>
       <c r="I176" t="n">
@@ -9704,7 +9704,7 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0177</t>
         </is>
       </c>
       <c r="I177" t="n">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0178</t>
         </is>
       </c>
       <c r="I178" t="n">
@@ -9806,7 +9806,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0179</t>
         </is>
       </c>
       <c r="I179" t="n">
@@ -9859,7 +9859,7 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0180</t>
         </is>
       </c>
       <c r="I180" t="n">
@@ -9910,7 +9910,7 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0181</t>
         </is>
       </c>
       <c r="I181" t="n">
@@ -9961,7 +9961,7 @@
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0182</t>
         </is>
       </c>
       <c r="I182" t="n">
@@ -10012,7 +10012,7 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0183</t>
         </is>
       </c>
       <c r="I183" t="n">
@@ -10064,7 +10064,7 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0184</t>
         </is>
       </c>
       <c r="I184" t="n">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0185</t>
         </is>
       </c>
       <c r="I185" t="n">
@@ -10166,7 +10166,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0186</t>
         </is>
       </c>
       <c r="I186" t="n">
@@ -10217,7 +10217,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0187</t>
         </is>
       </c>
       <c r="I187" t="n">
@@ -10268,7 +10268,7 @@
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0188</t>
         </is>
       </c>
       <c r="I188" t="n">
@@ -10319,7 +10319,7 @@
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0189</t>
         </is>
       </c>
       <c r="I189" t="n">
@@ -10372,7 +10372,7 @@
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0190</t>
         </is>
       </c>
       <c r="I190" t="n">
@@ -10425,7 +10425,7 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0191</t>
         </is>
       </c>
       <c r="I191" t="n">
@@ -10476,7 +10476,7 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0192</t>
         </is>
       </c>
       <c r="I192" t="n">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0193</t>
         </is>
       </c>
       <c r="I193" t="n">
@@ -10582,7 +10582,7 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0194</t>
         </is>
       </c>
       <c r="I194" t="n">
@@ -10635,7 +10635,7 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0195</t>
         </is>
       </c>
       <c r="I195" t="n">
@@ -10686,7 +10686,7 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0196</t>
         </is>
       </c>
       <c r="I196" t="n">
@@ -10737,7 +10737,7 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>FRC-7-S-22-0001</t>
+          <t>FRC-HQ-SLM-S-22-0197</t>
         </is>
       </c>
       <c r="I197" t="n">
@@ -10790,7 +10790,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0001</t>
+          <t>FRC-HQ-SLM-E-22-0198</t>
         </is>
       </c>
       <c r="I198" t="n">
@@ -10843,7 +10843,7 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0001</t>
+          <t>FRC-HQ-SLM-E-22-0199</t>
         </is>
       </c>
       <c r="I199" t="n">
@@ -10896,7 +10896,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0200</t>
         </is>
       </c>
       <c r="I200" t="n">
@@ -10949,7 +10949,7 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0201</t>
         </is>
       </c>
       <c r="I201" t="n">
@@ -11002,7 +11002,7 @@
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0202</t>
         </is>
       </c>
       <c r="I202" t="n">
@@ -11055,7 +11055,7 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0203</t>
         </is>
       </c>
       <c r="I203" t="n">
@@ -11108,7 +11108,7 @@
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0204</t>
         </is>
       </c>
       <c r="I204" t="n">
@@ -11161,7 +11161,7 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0205</t>
         </is>
       </c>
       <c r="I205" t="n">
@@ -11214,7 +11214,7 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0206</t>
         </is>
       </c>
       <c r="I206" t="n">
@@ -11267,7 +11267,7 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0207</t>
         </is>
       </c>
       <c r="I207" t="n">
@@ -11320,7 +11320,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0208</t>
         </is>
       </c>
       <c r="I208" t="n">
@@ -11373,7 +11373,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0209</t>
         </is>
       </c>
       <c r="I209" t="n">
@@ -11426,7 +11426,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0210</t>
         </is>
       </c>
       <c r="I210" t="n">
@@ -11479,7 +11479,7 @@
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0211</t>
         </is>
       </c>
       <c r="I211" t="n">
@@ -11532,7 +11532,7 @@
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0212</t>
         </is>
       </c>
       <c r="I212" t="n">
@@ -11585,7 +11585,7 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0213</t>
         </is>
       </c>
       <c r="I213" t="n">
@@ -11638,7 +11638,7 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0214</t>
         </is>
       </c>
       <c r="I214" t="n">
@@ -11691,7 +11691,7 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0215</t>
         </is>
       </c>
       <c r="I215" t="n">
@@ -11744,7 +11744,7 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0216</t>
         </is>
       </c>
       <c r="I216" t="n">
@@ -11797,7 +11797,7 @@
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0217</t>
         </is>
       </c>
       <c r="I217" t="n">
@@ -11850,7 +11850,7 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0218</t>
         </is>
       </c>
       <c r="I218" t="n">
@@ -11903,7 +11903,7 @@
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0219</t>
         </is>
       </c>
       <c r="I219" t="n">
@@ -11956,7 +11956,7 @@
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0220</t>
         </is>
       </c>
       <c r="I220" t="n">
@@ -12007,7 +12007,7 @@
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0221</t>
         </is>
       </c>
       <c r="I221" t="n">
@@ -12058,7 +12058,7 @@
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0222</t>
         </is>
       </c>
       <c r="I222" t="n">
@@ -12109,7 +12109,7 @@
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0223</t>
         </is>
       </c>
       <c r="I223" t="n">
@@ -12160,7 +12160,7 @@
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0224</t>
         </is>
       </c>
       <c r="I224" t="n">
@@ -12211,7 +12211,7 @@
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0225</t>
         </is>
       </c>
       <c r="I225" t="n">
@@ -12262,7 +12262,7 @@
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0226</t>
         </is>
       </c>
       <c r="I226" t="n">
@@ -12315,7 +12315,7 @@
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0227</t>
         </is>
       </c>
       <c r="I227" t="n">
@@ -12366,7 +12366,7 @@
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0228</t>
         </is>
       </c>
       <c r="I228" t="n">
@@ -12417,7 +12417,7 @@
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0229</t>
         </is>
       </c>
       <c r="I229" t="n">
@@ -12468,7 +12468,7 @@
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0230</t>
         </is>
       </c>
       <c r="I230" t="n">
@@ -12519,7 +12519,7 @@
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0231</t>
         </is>
       </c>
       <c r="I231" t="n">
@@ -12570,7 +12570,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0232</t>
         </is>
       </c>
       <c r="I232" t="n">
@@ -12621,7 +12621,7 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0233</t>
         </is>
       </c>
       <c r="I233" t="n">
@@ -12672,7 +12672,7 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0234</t>
         </is>
       </c>
       <c r="I234" t="n">
@@ -12723,7 +12723,7 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0235</t>
         </is>
       </c>
       <c r="I235" t="n">
@@ -12774,7 +12774,7 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>FRC-7-E-22-0002</t>
+          <t>FRC-HQ-SLM-E-22-0236</t>
         </is>
       </c>
       <c r="I236" t="n">
@@ -12825,7 +12825,7 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>FRC-7-P-22-0002</t>
+          <t>FRC-HQ-SLM-P-22-0237</t>
         </is>
       </c>
       <c r="I237" t="n">
@@ -12876,7 +12876,7 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>FRC-7-P-22-0002</t>
+          <t>FRC-HQ-SLM-P-22-0238</t>
         </is>
       </c>
       <c r="I238" t="n">
@@ -12927,7 +12927,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>FRC-7-P-22-0002</t>
+          <t>FRC-HQ-SLM-P-22-0239</t>
         </is>
       </c>
       <c r="I239" t="n">
@@ -12978,7 +12978,7 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>FRC-7-P-22-0002</t>
+          <t>FRC-HQ-SLM-P-22-0240</t>
         </is>
       </c>
       <c r="I240" t="n">
@@ -13029,7 +13029,7 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>FRC-7-P-22-0002</t>
+          <t>FRC-HQ-SLM-P-22-0241</t>
         </is>
       </c>
       <c r="I241" t="n">
@@ -13080,7 +13080,7 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0242</t>
         </is>
       </c>
       <c r="I242" t="n">
@@ -13131,7 +13131,7 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0243</t>
         </is>
       </c>
       <c r="I243" t="n">
@@ -13182,7 +13182,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0244</t>
         </is>
       </c>
       <c r="I244" t="n">
@@ -13233,7 +13233,7 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0245</t>
         </is>
       </c>
       <c r="I245" t="n">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0246</t>
         </is>
       </c>
       <c r="I246" t="n">
@@ -13335,7 +13335,7 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0247</t>
         </is>
       </c>
       <c r="I247" t="n">
@@ -13386,7 +13386,7 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0248</t>
         </is>
       </c>
       <c r="I248" t="n">
@@ -13437,7 +13437,7 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0249</t>
         </is>
       </c>
       <c r="I249" t="n">
@@ -13488,7 +13488,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0250</t>
         </is>
       </c>
       <c r="I250" t="n">
@@ -13539,7 +13539,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0251</t>
         </is>
       </c>
       <c r="I251" t="n">
@@ -13590,7 +13590,7 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0252</t>
         </is>
       </c>
       <c r="I252" t="n">
@@ -13641,7 +13641,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0253</t>
         </is>
       </c>
       <c r="I253" t="n">
@@ -13692,7 +13692,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0254</t>
         </is>
       </c>
       <c r="I254" t="n">
@@ -13743,7 +13743,7 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0255</t>
         </is>
       </c>
       <c r="I255" t="n">
@@ -13794,7 +13794,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0256</t>
         </is>
       </c>
       <c r="I256" t="n">
@@ -13845,7 +13845,7 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0257</t>
         </is>
       </c>
       <c r="I257" t="n">
@@ -13896,7 +13896,7 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0258</t>
         </is>
       </c>
       <c r="I258" t="n">
@@ -13947,7 +13947,7 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0259</t>
         </is>
       </c>
       <c r="I259" t="n">
@@ -13998,7 +13998,7 @@
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0260</t>
         </is>
       </c>
       <c r="I260" t="n">
@@ -14049,7 +14049,7 @@
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0261</t>
         </is>
       </c>
       <c r="I261" t="n">
@@ -14100,7 +14100,7 @@
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0262</t>
         </is>
       </c>
       <c r="I262" t="n">
@@ -14151,7 +14151,7 @@
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0263</t>
         </is>
       </c>
       <c r="I263" t="n">
@@ -14202,7 +14202,7 @@
       </c>
       <c r="H264" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0264</t>
         </is>
       </c>
       <c r="I264" t="n">
@@ -14253,7 +14253,7 @@
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0265</t>
         </is>
       </c>
       <c r="I265" t="n">
@@ -14304,7 +14304,7 @@
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0266</t>
         </is>
       </c>
       <c r="I266" t="n">
@@ -14355,7 +14355,7 @@
       </c>
       <c r="H267" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0267</t>
         </is>
       </c>
       <c r="I267" t="n">
@@ -14406,7 +14406,7 @@
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0268</t>
         </is>
       </c>
       <c r="I268" t="n">
@@ -14457,7 +14457,7 @@
       </c>
       <c r="H269" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0269</t>
         </is>
       </c>
       <c r="I269" t="n">
@@ -14508,7 +14508,7 @@
       </c>
       <c r="H270" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0270</t>
         </is>
       </c>
       <c r="I270" t="n">
@@ -14559,7 +14559,7 @@
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0271</t>
         </is>
       </c>
       <c r="I271" t="n">
@@ -14610,7 +14610,7 @@
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0272</t>
         </is>
       </c>
       <c r="I272" t="n">
@@ -14661,7 +14661,7 @@
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0273</t>
         </is>
       </c>
       <c r="I273" t="n">
@@ -14712,7 +14712,7 @@
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>FRC-7-I-22-0002</t>
+          <t>FRC-HQ-SLM-I-22-0274</t>
         </is>
       </c>
       <c r="I274" t="n">
@@ -14763,7 +14763,7 @@
       </c>
       <c r="H275" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0275</t>
         </is>
       </c>
       <c r="I275" t="n">
@@ -14814,7 +14814,7 @@
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0276</t>
         </is>
       </c>
       <c r="I276" t="n">
@@ -14865,7 +14865,7 @@
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0277</t>
         </is>
       </c>
       <c r="I277" t="n">
@@ -14916,7 +14916,7 @@
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0278</t>
         </is>
       </c>
       <c r="I278" t="n">
@@ -14967,7 +14967,7 @@
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0279</t>
         </is>
       </c>
       <c r="I279" t="n">
@@ -15018,7 +15018,7 @@
       </c>
       <c r="H280" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0280</t>
         </is>
       </c>
       <c r="I280" t="n">
@@ -15069,7 +15069,7 @@
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0281</t>
         </is>
       </c>
       <c r="I281" t="n">
@@ -15120,7 +15120,7 @@
       </c>
       <c r="H282" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0282</t>
         </is>
       </c>
       <c r="I282" t="n">
@@ -15171,7 +15171,7 @@
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0283</t>
         </is>
       </c>
       <c r="I283" t="n">
@@ -15224,7 +15224,7 @@
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0284</t>
         </is>
       </c>
       <c r="I284" t="n">
@@ -15277,7 +15277,7 @@
       </c>
       <c r="H285" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0285</t>
         </is>
       </c>
       <c r="I285" t="n">
@@ -15330,7 +15330,7 @@
       </c>
       <c r="H286" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0286</t>
         </is>
       </c>
       <c r="I286" t="n">
@@ -15381,7 +15381,7 @@
       </c>
       <c r="H287" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0287</t>
         </is>
       </c>
       <c r="I287" t="n">
@@ -15434,7 +15434,7 @@
       </c>
       <c r="H288" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0288</t>
         </is>
       </c>
       <c r="I288" t="n">
@@ -15487,7 +15487,7 @@
       </c>
       <c r="H289" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0289</t>
         </is>
       </c>
       <c r="I289" t="n">
@@ -15540,7 +15540,7 @@
       </c>
       <c r="H290" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0290</t>
         </is>
       </c>
       <c r="I290" t="n">
@@ -15593,7 +15593,7 @@
       </c>
       <c r="H291" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0291</t>
         </is>
       </c>
       <c r="I291" t="n">
@@ -15646,7 +15646,7 @@
       </c>
       <c r="H292" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0292</t>
         </is>
       </c>
       <c r="I292" t="n">
@@ -15699,7 +15699,7 @@
       </c>
       <c r="H293" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0293</t>
         </is>
       </c>
       <c r="I293" t="n">
@@ -15752,7 +15752,7 @@
       </c>
       <c r="H294" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0294</t>
         </is>
       </c>
       <c r="I294" t="n">
@@ -15805,7 +15805,7 @@
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0295</t>
         </is>
       </c>
       <c r="I295" t="n">
@@ -15856,7 +15856,7 @@
       </c>
       <c r="H296" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0296</t>
         </is>
       </c>
       <c r="I296" t="n">
@@ -15907,7 +15907,7 @@
       </c>
       <c r="H297" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0297</t>
         </is>
       </c>
       <c r="I297" t="n">
@@ -15958,7 +15958,7 @@
       </c>
       <c r="H298" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0298</t>
         </is>
       </c>
       <c r="I298" t="n">
@@ -16009,7 +16009,7 @@
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0002</t>
+          <t>FRC-HQ-SLM-F-22-0299</t>
         </is>
       </c>
       <c r="I299" t="n">
@@ -16060,7 +16060,7 @@
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0003</t>
+          <t>FRC-HQ-SLM-F-22-0300</t>
         </is>
       </c>
       <c r="I300" t="n">
@@ -16111,7 +16111,7 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>FRC-7-F-22-0003</t>
+          <t>FRC-HQ-SLM-F-22-0301</t>
         </is>
       </c>
       <c r="I301" t="n">

</xml_diff>